<commit_message>
Creating a new inventory screen based on GameDevelopmentCenter tutorial 1
-- imported several fonts and textures (probably more than needed)
-- Redesigned the inventory screen prototype. Removed all inventory functionality for now.
-- may need to choose a different background, border, and font type for this.
-- added JSON data for a test loot table
</commit_message>
<xml_diff>
--- a/resources/data/LootTable.xlsx
+++ b/resources/data/LootTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\_GAME_DEVELOP\New-Duhamell\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56C68FA6-252A-4DC8-BFE2-C77014D065AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66444A1-5E8F-4AB8-82BD-455B4CF770AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="570" windowWidth="27795" windowHeight="15000" xr2:uid="{DA5CD4F1-CFA9-4461-8D9F-C62446E768BC}"/>
+    <workbookView xWindow="2355" yWindow="1050" windowWidth="27795" windowHeight="15000" xr2:uid="{DA5CD4F1-CFA9-4461-8D9F-C62446E768BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>MapName</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Iron Ore</t>
+  </si>
+  <si>
+    <t>ItemCountMin</t>
+  </si>
+  <si>
+    <t>ItemCountMax</t>
   </si>
 </sst>
 </file>
@@ -467,215 +473,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEE1858-40D8-4A2B-A44F-630C8F8BA78D}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>80</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>15</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
       <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>70</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>20</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>15</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>25</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>15</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>60</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>45</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>120</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>30</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>10</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
State machine fixes for monster behavior.
- Individual states now exist as separate node entities.
- code clean up and some refactoring.
</commit_message>
<xml_diff>
--- a/resources/data/LootTable.xlsx
+++ b/resources/data/LootTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\_GAME_DEVELOP\New-Duhamell\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66444A1-5E8F-4AB8-82BD-455B4CF770AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366A7AC3-8140-4B7A-939E-D52B9831B766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="1050" windowWidth="27795" windowHeight="15000" xr2:uid="{DA5CD4F1-CFA9-4461-8D9F-C62446E768BC}"/>
+    <workbookView xWindow="-20655" yWindow="1215" windowWidth="46935" windowHeight="15000" xr2:uid="{DA5CD4F1-CFA9-4461-8D9F-C62446E768BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>MapName</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>ItemCountMax</t>
+  </si>
+  <si>
+    <t>Item3Name</t>
+  </si>
+  <si>
+    <t>Iron Cuirass</t>
+  </si>
+  <si>
+    <t>Iron Boots</t>
+  </si>
+  <si>
+    <t>Iron Spear</t>
   </si>
 </sst>
 </file>
@@ -473,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEE1858-40D8-4A2B-A44F-630C8F8BA78D}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="Q2" sqref="Q2:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -492,12 +504,13 @@
     <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.125" customWidth="1"/>
+    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,16 +545,19 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -575,17 +591,24 @@
       <c r="K2">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
         <v>5</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
         <v>1</v>
       </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>_xlfn.CONCAT("{",CHAR(34),$A$1,CHAR(34),":",CHAR(34),$A2,CHAR(34),",",CHAR(34),$B$1,CHAR(34),":",CHAR(34),$B2,CHAR(34),",",CHAR(34),$C$1,CHAR(34),":",CHAR(34),$C2,CHAR(34),",",CHAR(34),$D$1,CHAR(34),":",CHAR(34),$D2,CHAR(34),",",CHAR(34),$E$1,CHAR(34),":",CHAR(34),$E2,CHAR(34),",",CHAR(34),$F$1,CHAR(34),":",CHAR(34),$F2,CHAR(34),",",CHAR(34),$G$1,CHAR(34),":",CHAR(34),$G2,CHAR(34),",",CHAR(34),$H$1,CHAR(34),":",CHAR(34),$H2,CHAR(34),",",CHAR(34),$I$1,CHAR(34),":",CHAR(34),$I2,CHAR(34),",",CHAR(34),$J$1,CHAR(34),":",CHAR(34),$J2,CHAR(34),",",CHAR(34),$K$1,CHAR(34),":",CHAR(34),$K2,CHAR(34),",",CHAR(34),$L$1,CHAR(34),":",CHAR(34),$L2,CHAR(34),",",CHAR(34),$M$1,CHAR(34),":",CHAR(34),$M2,CHAR(34),",",CHAR(34),$N$1,CHAR(34),":",CHAR(34),$N2,CHAR(34),",",CHAR(34),$O$1,CHAR(34),":",CHAR(34),$O2,CHAR(34),"},")</f>
+        <v>{"MapName":"Tutorial1","ItemCountMin":"1","ItemCountMax":"2","Item1Name":"Gold","Item1Chance":"80","Item1MinQ":"2","Item1MaxQ":"5","Item2Name":"Iron Sword","Item2Chance":"15","Item2MinQ":"1","Item2MaxQ":"1","Item3Name":"Iron Cuirass","Item3Chance":"5","Item3MinQ":"1","Item3MaxQ":"1"},</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -619,17 +642,24 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3">
         <v>10</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
         <v>1</v>
       </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q5" si="0">_xlfn.CONCAT("{",CHAR(34),$A$1,CHAR(34),":",CHAR(34),$A3,CHAR(34),",",CHAR(34),$B$1,CHAR(34),":",CHAR(34),$B3,CHAR(34),",",CHAR(34),$C$1,CHAR(34),":",CHAR(34),$C3,CHAR(34),",",CHAR(34),$D$1,CHAR(34),":",CHAR(34),$D3,CHAR(34),",",CHAR(34),$E$1,CHAR(34),":",CHAR(34),$E3,CHAR(34),",",CHAR(34),$F$1,CHAR(34),":",CHAR(34),$F3,CHAR(34),",",CHAR(34),$G$1,CHAR(34),":",CHAR(34),$G3,CHAR(34),",",CHAR(34),$H$1,CHAR(34),":",CHAR(34),$H3,CHAR(34),",",CHAR(34),$I$1,CHAR(34),":",CHAR(34),$I3,CHAR(34),",",CHAR(34),$J$1,CHAR(34),":",CHAR(34),$J3,CHAR(34),",",CHAR(34),$K$1,CHAR(34),":",CHAR(34),$K3,CHAR(34),",",CHAR(34),$L$1,CHAR(34),":",CHAR(34),$L3,CHAR(34),",",CHAR(34),$M$1,CHAR(34),":",CHAR(34),$M3,CHAR(34),",",CHAR(34),$N$1,CHAR(34),":",CHAR(34),$N3,CHAR(34),",",CHAR(34),$O$1,CHAR(34),":",CHAR(34),$O3,CHAR(34),"},")</f>
+        <v>{"MapName":"Tutorial2","ItemCountMin":"1","ItemCountMax":"2","Item1Name":"Gold","Item1Chance":"70","Item1MinQ":"2","Item1MaxQ":"5","Item2Name":"Iron Sword","Item2Chance":"20","Item2MinQ":"1","Item2MaxQ":"1","Item3Name":"Iron Cuirass","Item3Chance":"10","Item3MinQ":"1","Item3MaxQ":"1"},</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -663,17 +693,24 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
         <v>1</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="0"/>
+        <v>{"MapName":"Grassland1","ItemCountMin":"1","ItemCountMax":"3","Item1Name":"Gold","Item1Chance":"60","Item1MinQ":"15","Item1MaxQ":"35","Item2Name":"Steel Sword","Item2Chance":"25","Item2MinQ":"1","Item2MaxQ":"1","Item3Name":"Iron Boots","Item3Chance":"15","Item3MinQ":"1","Item3MaxQ":"1"},</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -707,17 +744,25 @@
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5">
         <v>10</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
       <c r="N5">
         <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="0"/>
+        <v>{"MapName":"Grassland2","ItemCountMin":"1","ItemCountMax":"3","Item1Name":"Gold","Item1Chance":"60","Item1MinQ":"45","Item1MaxQ":"120","Item2Name":"Iron Ore","Item2Chance":"30","Item2MinQ":"1","Item2MaxQ":"3","Item3Name":"Iron Spear","Item3Chance":"10","Item3MinQ":"1","Item3MaxQ":"1"},</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>